<commit_message>
Updated version through JSON
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="74">
   <si>
     <t>RECORD_ID</t>
   </si>
@@ -237,6 +237,18 @@
   </si>
   <si>
     <t>2398jw</t>
+  </si>
+  <si>
+    <t>0615037491</t>
+  </si>
+  <si>
+    <t>0633319950</t>
+  </si>
+  <si>
+    <t>0383319349</t>
+  </si>
+  <si>
+    <t>003138426401</t>
   </si>
 </sst>
 </file>
@@ -281,9 +293,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -565,12 +578,13 @@
   <dimension ref="A1:Q10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="21.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -649,8 +663,8 @@
       <c r="I2" t="s">
         <v>52</v>
       </c>
-      <c r="J2">
-        <v>615037491</v>
+      <c r="J2" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>58</v>
@@ -684,8 +698,8 @@
       <c r="I3" t="s">
         <v>53</v>
       </c>
-      <c r="J3">
-        <v>633319950</v>
+      <c r="J3" s="2" t="s">
+        <v>71</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>59</v>
@@ -716,8 +730,8 @@
       <c r="I4" t="s">
         <v>54</v>
       </c>
-      <c r="J4">
-        <v>383319349</v>
+      <c r="J4" s="2" t="s">
+        <v>72</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>60</v>
@@ -747,6 +761,9 @@
       </c>
       <c r="I5" t="s">
         <v>68</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>73</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>61</v>

</xml_diff>